<commit_message>
Regenerate Gerbers using PCBWay process
</commit_message>
<xml_diff>
--- a/Fabrication/Canary-BOM-processed.xlsx
+++ b/Fabrication/Canary-BOM-processed.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\KiCAD\Canary\Fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4AF2B3-2634-4625-8AD0-3459D713E44B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B623501-D7CF-4171-8CD4-AF0A109387C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="50505" windowHeight="28067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Canary-BOM-raw" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="214">
   <si>
     <t>Reference(s)</t>
   </si>
@@ -659,6 +670,9 @@
   </si>
   <si>
     <t>Component Count:</t>
+  </si>
+  <si>
+    <t>Populated Component Count:</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2597,6 +2611,19 @@
         <v>97</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="1">
+        <f>B64-SUM(C47:C58)</f>
+        <v>77</v>
+      </c>
+      <c r="C66">
+        <f>SUM(Table1[Qty])</f>
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>